<commit_message>
To address first round reveiwer comments and add conjugated LCA
</commit_message>
<xml_diff>
--- a/Excel Exports/Table S4.xlsx
+++ b/Excel Exports/Table S4.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -436,7 +436,7 @@
         <v>2.07634104183089e-12</v>
       </c>
       <c r="I2">
-        <v>1.91023375848442e-10</v>
+        <v>2.15939468350412e-10</v>
       </c>
     </row>
     <row r="3">
@@ -471,7 +471,7 @@
         <v>4.202198577965539e-12</v>
       </c>
       <c r="I3">
-        <v>3.866022691728301e-10</v>
+        <v>4.37028652108416e-10</v>
       </c>
     </row>
     <row r="4">
@@ -506,7 +506,7 @@
         <v>1.45437444646967e-11</v>
       </c>
       <c r="I4">
-        <v>1.3380244907521e-09</v>
+        <v>1.51254942432846e-09</v>
       </c>
     </row>
     <row r="5">
@@ -541,7 +541,7 @@
         <v>1.20183607568749e-10</v>
       </c>
       <c r="I5">
-        <v>1.10568918963249e-08</v>
+        <v>1.24990951871499e-08</v>
       </c>
     </row>
     <row r="6">
@@ -576,7 +576,7 @@
         <v>1.40436521540901e-10</v>
       </c>
       <c r="I6">
-        <v>1.29201599817629e-08</v>
+        <v>1.46053982402537e-08</v>
       </c>
     </row>
     <row r="7">
@@ -611,7 +611,7 @@
         <v>4.61325902243821e-10</v>
       </c>
       <c r="I7">
-        <v>4.24419830064315e-08</v>
+        <v>4.79778938333574e-08</v>
       </c>
     </row>
     <row r="8">
@@ -646,7 +646,7 @@
         <v>2.75202020614045e-09</v>
       </c>
       <c r="I8">
-        <v>2.53185858964922e-07</v>
+        <v>2.86210101438607e-07</v>
       </c>
     </row>
     <row r="9">
@@ -681,7 +681,7 @@
         <v>3.11625182054012e-07</v>
       </c>
       <c r="I9">
-        <v>2.86695167489691e-05</v>
+        <v>3.24090189336173e-05</v>
       </c>
     </row>
     <row r="10">
@@ -716,7 +716,7 @@
         <v>4.5984608362644e-07</v>
       </c>
       <c r="I10">
-        <v>4.23058396936325e-05</v>
+        <v>4.78239926971498e-05</v>
       </c>
     </row>
     <row r="11">
@@ -751,7 +751,7 @@
         <v>5.67305064688184e-07</v>
       </c>
       <c r="I11">
-        <v>5.21920659513129e-05</v>
+        <v>5.89997267275712e-05</v>
       </c>
     </row>
     <row r="12">
@@ -786,7 +786,7 @@
         <v>7.59518768878836e-07</v>
       </c>
       <c r="I12">
-        <v>6.98757267368529e-05</v>
+        <v>7.89899519633989e-05</v>
       </c>
     </row>
     <row r="13">
@@ -821,7 +821,7 @@
         <v>7.83677990653401e-07</v>
       </c>
       <c r="I13">
-        <v>7.20983751401129e-05</v>
+        <v>8.15025110279537e-05</v>
       </c>
     </row>
     <row r="14">
@@ -856,13 +856,13 @@
         <v>1.44290737102832e-06</v>
       </c>
       <c r="I14">
-        <v>0.0001327474781346</v>
+        <v>0.00015006236658694</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Phe_DCA</t>
+          <t>Phe_LCA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -876,28 +876,28 @@
         </is>
       </c>
       <c r="D15">
-        <v>5.61230382894244</v>
+        <v>3.14892084911381</v>
       </c>
       <c r="E15">
-        <v>1.00538062147341</v>
+        <v>0.549405518745987</v>
       </c>
       <c r="F15">
         <v>45</v>
       </c>
       <c r="G15">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H15">
-        <v>3.4344786525092e-06</v>
+        <v>2.12799556778026e-06</v>
       </c>
       <c r="I15">
-        <v>0.00031597203603084</v>
+        <v>0.00022131153904914</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ala_CA</t>
+          <t>Phe_DCA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -911,28 +911,28 @@
         </is>
       </c>
       <c r="D16">
-        <v>-3.99440097149882</v>
+        <v>5.61230382894244</v>
       </c>
       <c r="E16">
-        <v>0.7307283688026039</v>
+        <v>1.00538062147341</v>
       </c>
       <c r="F16">
         <v>45</v>
       </c>
       <c r="G16">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H16">
-        <v>5.50427918786294e-06</v>
+        <v>3.4344786525092e-06</v>
       </c>
       <c r="I16">
-        <v>0.00050639368528339</v>
+        <v>0.00035718577986095</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>aMCA</t>
+          <t>Leu_LCA</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -946,28 +946,28 @@
         </is>
       </c>
       <c r="D17">
-        <v>6.02194339282892</v>
+        <v>4.50343040381207</v>
       </c>
       <c r="E17">
-        <v>1.08790042964967</v>
+        <v>0.809935656636282</v>
       </c>
       <c r="F17">
         <v>45</v>
       </c>
       <c r="G17">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="H17">
-        <v>6.79441236759733e-06</v>
+        <v>4.41108738251035e-06</v>
       </c>
       <c r="I17">
-        <v>0.00062508593781895</v>
+        <v>0.00045875308778107</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ala_CDCA</t>
+          <t>Ala_CA</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -981,28 +981,28 @@
         </is>
       </c>
       <c r="D18">
-        <v>-3.56294420349548</v>
+        <v>-3.99440097149882</v>
       </c>
       <c r="E18">
-        <v>0.65534971132165</v>
+        <v>0.7307283688026039</v>
       </c>
       <c r="F18">
         <v>45</v>
       </c>
       <c r="G18">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H18">
-        <v>7.29153248337249e-06</v>
+        <v>5.50427918786294e-06</v>
       </c>
       <c r="I18">
-        <v>0.00067082098847026</v>
+        <v>0.0005724450355377401</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Ser_CDCA</t>
+          <t>aMCA</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1016,28 +1016,28 @@
         </is>
       </c>
       <c r="D19">
-        <v>-3.632099392129</v>
+        <v>6.02194339282892</v>
       </c>
       <c r="E19">
-        <v>0.663847929040851</v>
+        <v>1.08790042964967</v>
       </c>
       <c r="F19">
         <v>45</v>
       </c>
       <c r="G19">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H19">
-        <v>7.7577106468652e-06</v>
+        <v>6.79441236759733e-06</v>
       </c>
       <c r="I19">
-        <v>0.00071370937951159</v>
+        <v>0.00070661888623012</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ala_DCA</t>
+          <t>Ala_CDCA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1051,28 +1051,28 @@
         </is>
       </c>
       <c r="D20">
-        <v>3.89548478573192</v>
+        <v>-3.56294420349548</v>
       </c>
       <c r="E20">
-        <v>0.7494068893904871</v>
+        <v>0.65534971132165</v>
       </c>
       <c r="F20">
         <v>45</v>
       </c>
       <c r="G20">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H20">
-        <v>9.76733032826185e-06</v>
+        <v>7.29153248337249e-06</v>
       </c>
       <c r="I20">
-        <v>0.00089859439020009</v>
+        <v>0.00075831937827073</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GCA</t>
+          <t>Ser_CDCA</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1086,28 +1086,28 @@
         </is>
       </c>
       <c r="D21">
-        <v>-4.92580700744384</v>
+        <v>-3.632099392129</v>
       </c>
       <c r="E21">
-        <v>0.995256441604661</v>
+        <v>0.663847929040851</v>
       </c>
       <c r="F21">
         <v>45</v>
       </c>
       <c r="G21">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="H21">
-        <v>1.19496295993144e-05</v>
+        <v>7.7577106468652e-06</v>
       </c>
       <c r="I21">
-        <v>0.00109936592313692</v>
+        <v>0.00080680190727398</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GHCA</t>
+          <t>Ala_DCA</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1121,28 +1121,28 @@
         </is>
       </c>
       <c r="D22">
-        <v>-4.05668590968884</v>
+        <v>3.89548478573192</v>
       </c>
       <c r="E22">
-        <v>0.824094961079904</v>
+        <v>0.7494068893904871</v>
       </c>
       <c r="F22">
         <v>45</v>
       </c>
       <c r="G22">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H22">
-        <v>1.30381666742032e-05</v>
+        <v>9.76733032826185e-06</v>
       </c>
       <c r="I22">
-        <v>0.00119951133402669</v>
+        <v>0.00101580235413923</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TCDCA</t>
+          <t>GCA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1156,28 +1156,28 @@
         </is>
       </c>
       <c r="D23">
-        <v>-5.09482588071409</v>
+        <v>-4.92580700744384</v>
       </c>
       <c r="E23">
-        <v>0.990301292817899</v>
+        <v>0.995256441604661</v>
       </c>
       <c r="F23">
         <v>45</v>
       </c>
       <c r="G23">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H23">
-        <v>1.44996488621762e-05</v>
+        <v>1.19496295993144e-05</v>
       </c>
       <c r="I23">
-        <v>0.00133396769532021</v>
+        <v>0.00124276147832869</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>TaMCA</t>
+          <t>GHCA</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1191,10 +1191,10 @@
         </is>
       </c>
       <c r="D24">
-        <v>-3.01474686871361</v>
+        <v>-4.05668590968884</v>
       </c>
       <c r="E24">
-        <v>0.617663520649549</v>
+        <v>0.824094961079904</v>
       </c>
       <c r="F24">
         <v>45</v>
@@ -1203,16 +1203,16 @@
         <v>12</v>
       </c>
       <c r="H24">
-        <v>1.4938107058691e-05</v>
+        <v>1.30381666742032e-05</v>
       </c>
       <c r="I24">
-        <v>0.00137430584939957</v>
+        <v>0.00135596933411713</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CDCA</t>
+          <t>TCDCA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1226,28 +1226,28 @@
         </is>
       </c>
       <c r="D25">
-        <v>-3.44218225536413</v>
+        <v>-5.09482588071409</v>
       </c>
       <c r="E25">
-        <v>0.701033069714713</v>
+        <v>0.990301292817899</v>
       </c>
       <c r="F25">
         <v>45</v>
       </c>
       <c r="G25">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H25">
-        <v>2.3396087777826e-05</v>
+        <v>1.44996488621762e-05</v>
       </c>
       <c r="I25">
-        <v>0.00215244007555999</v>
+        <v>0.00150796348166633</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>His_CA</t>
+          <t>TaMCA</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1261,28 +1261,28 @@
         </is>
       </c>
       <c r="D26">
-        <v>-4.13578530660973</v>
+        <v>-3.01474686871361</v>
       </c>
       <c r="E26">
-        <v>0.887026283907809</v>
+        <v>0.617663520649549</v>
       </c>
       <c r="F26">
         <v>45</v>
       </c>
       <c r="G26">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H26">
-        <v>3.03187383528187e-05</v>
+        <v>1.4938107058691e-05</v>
       </c>
       <c r="I26">
-        <v>0.00278932392845932</v>
+        <v>0.00155356313410387</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Phe_CDCA</t>
+          <t>Trp_LCA</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1296,28 +1296,28 @@
         </is>
       </c>
       <c r="D27">
-        <v>-4.53213492034046</v>
+        <v>3.46232069014383</v>
       </c>
       <c r="E27">
-        <v>0.956395029881575</v>
+        <v>0.701548503447427</v>
       </c>
       <c r="F27">
         <v>45</v>
       </c>
       <c r="G27">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H27">
-        <v>4.03003950944963e-05</v>
+        <v>2.11615096898017e-05</v>
       </c>
       <c r="I27">
-        <v>0.00370763634869366</v>
+        <v>0.00220079700773937</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Ile_Leu_DCA</t>
+          <t>CDCA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1331,28 +1331,28 @@
         </is>
       </c>
       <c r="D28">
-        <v>5.23378121321908</v>
+        <v>-3.44218225536413</v>
       </c>
       <c r="E28">
-        <v>1.09137294835263</v>
+        <v>0.701033069714713</v>
       </c>
       <c r="F28">
         <v>45</v>
       </c>
       <c r="G28">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="H28">
-        <v>4.31441836206151e-05</v>
+        <v>2.3396087777826e-05</v>
       </c>
       <c r="I28">
-        <v>0.00396926489309659</v>
+        <v>0.0024331931288939</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Phe_CA</t>
+          <t>Val_LCA</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1366,10 +1366,10 @@
         </is>
       </c>
       <c r="D29">
-        <v>-6.72489423000699</v>
+        <v>3.6680099388394</v>
       </c>
       <c r="E29">
-        <v>1.44636676409151</v>
+        <v>0.745300632001675</v>
       </c>
       <c r="F29">
         <v>45</v>
@@ -1378,16 +1378,16 @@
         <v>22</v>
       </c>
       <c r="H29">
-        <v>5.16130324883337e-05</v>
+        <v>2.3852244711171e-05</v>
       </c>
       <c r="I29">
-        <v>0.0047483989889267</v>
+        <v>0.00248063344996179</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ile_Leu_CDCA</t>
+          <t>His_CA</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1401,28 +1401,28 @@
         </is>
       </c>
       <c r="D30">
-        <v>-2.95590825629201</v>
+        <v>-4.13578530660973</v>
       </c>
       <c r="E30">
-        <v>0.668253345696835</v>
+        <v>0.887026283907809</v>
       </c>
       <c r="F30">
         <v>45</v>
       </c>
       <c r="G30">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H30">
-        <v>6.51992217470614e-05</v>
+        <v>3.03187383528187e-05</v>
       </c>
       <c r="I30">
-        <v>0.00599832840072965</v>
+        <v>0.00315314878869315</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Ser_CA</t>
+          <t>Phe_CDCA</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1436,28 +1436,28 @@
         </is>
       </c>
       <c r="D31">
-        <v>-3.75330853888372</v>
+        <v>-4.53213492034046</v>
       </c>
       <c r="E31">
-        <v>0.809489986563165</v>
+        <v>0.956395029881575</v>
       </c>
       <c r="F31">
         <v>45</v>
       </c>
       <c r="G31">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H31">
-        <v>7.78389994408589e-05</v>
+        <v>4.03003950944963e-05</v>
       </c>
       <c r="I31">
-        <v>0.00716118794855902</v>
+        <v>0.00419124108982762</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GCDCA</t>
+          <t>Ile_Leu_DCA</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1471,28 +1471,28 @@
         </is>
       </c>
       <c r="D32">
-        <v>-3.99439541513951</v>
+        <v>5.23378121321908</v>
       </c>
       <c r="E32">
-        <v>0.92685196707319</v>
+        <v>1.09137294835263</v>
       </c>
       <c r="F32">
         <v>45</v>
       </c>
       <c r="G32">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="H32">
-        <v>9.34373196423311e-05</v>
+        <v>4.31441836206151e-05</v>
       </c>
       <c r="I32">
-        <v>0.008596233407094461</v>
+        <v>0.00448699509654397</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Trp_DCA</t>
+          <t>Phe_CA</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1506,28 +1506,28 @@
         </is>
       </c>
       <c r="D33">
-        <v>3.8823258203524</v>
+        <v>-6.72489423000699</v>
       </c>
       <c r="E33">
-        <v>0.899046775504252</v>
+        <v>1.44636676409151</v>
       </c>
       <c r="F33">
         <v>45</v>
       </c>
       <c r="G33">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H33">
-        <v>0.0001329376744763</v>
+        <v>5.16130324883337e-05</v>
       </c>
       <c r="I33">
-        <v>0.0122302660518199</v>
+        <v>0.0053677553787867</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Tyr_DCA</t>
+          <t>Ile_Leu_CDCA</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1541,28 +1541,28 @@
         </is>
       </c>
       <c r="D34">
-        <v>3.7903619422196</v>
+        <v>-2.95590825629201</v>
       </c>
       <c r="E34">
-        <v>0.8787987909782931</v>
+        <v>0.668253345696835</v>
       </c>
       <c r="F34">
         <v>45</v>
       </c>
       <c r="G34">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H34">
-        <v>0.00013553825659997</v>
+        <v>6.51992217470614e-05</v>
       </c>
       <c r="I34">
-        <v>0.0124695196071975</v>
+        <v>0.00678071906169438</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>GLCA</t>
+          <t>Tyr_LCA</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1576,28 +1576,28 @@
         </is>
       </c>
       <c r="D35">
-        <v>4.49364453060249</v>
+        <v>-4.42283827279717</v>
       </c>
       <c r="E35">
-        <v>1.06465699673004</v>
+        <v>0.97598203039319</v>
       </c>
       <c r="F35">
         <v>45</v>
       </c>
       <c r="G35">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H35">
-        <v>0.00017803174137804</v>
+        <v>7.34752758994595e-05</v>
       </c>
       <c r="I35">
-        <v>0.0163789202067805</v>
+        <v>0.00764142869354379</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Lys_DCA_a</t>
+          <t>Ser_CA</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1611,28 +1611,28 @@
         </is>
       </c>
       <c r="D36">
-        <v>1.33609083935223</v>
+        <v>-3.75330853888372</v>
       </c>
       <c r="E36">
-        <v>0.318238128441892</v>
+        <v>0.809489986563165</v>
       </c>
       <c r="F36">
         <v>45</v>
       </c>
       <c r="G36">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H36">
-        <v>0.00018922025554688</v>
+        <v>7.78389994408589e-05</v>
       </c>
       <c r="I36">
-        <v>0.0174082635103135</v>
+        <v>0.00809525594184933</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>TbMCA</t>
+          <t>GCDCA</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1646,28 +1646,28 @@
         </is>
       </c>
       <c r="D37">
-        <v>-3.07838356838709</v>
+        <v>-3.99439541513951</v>
       </c>
       <c r="E37">
-        <v>0.720246856317878</v>
+        <v>0.92685196707319</v>
       </c>
       <c r="F37">
         <v>45</v>
       </c>
       <c r="G37">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="H37">
-        <v>0.00022260807418096</v>
+        <v>9.34373196423311e-05</v>
       </c>
       <c r="I37">
-        <v>0.020479942824649</v>
+        <v>0.009717481242802429</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Glu_DCA</t>
+          <t>Trp_DCA</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1681,10 +1681,10 @@
         </is>
       </c>
       <c r="D38">
-        <v>4.14453675934297</v>
+        <v>3.8823258203524</v>
       </c>
       <c r="E38">
-        <v>1.01797610844224</v>
+        <v>0.899046775504252</v>
       </c>
       <c r="F38">
         <v>45</v>
@@ -1693,16 +1693,16 @@
         <v>19</v>
       </c>
       <c r="H38">
-        <v>0.00026496332538166</v>
+        <v>0.0001329376744763</v>
       </c>
       <c r="I38">
-        <v>0.0243766259351134</v>
+        <v>0.0138255181455355</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>THDCA</t>
+          <t>Tyr_DCA</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1716,28 +1716,28 @@
         </is>
       </c>
       <c r="D39">
-        <v>-2.43236725452046</v>
+        <v>3.7903619422196</v>
       </c>
       <c r="E39">
-        <v>0.602796137501093</v>
+        <v>0.8787987909782931</v>
       </c>
       <c r="F39">
         <v>45</v>
       </c>
       <c r="G39">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="H39">
-        <v>0.00031170816337839</v>
+        <v>0.00013553825659997</v>
       </c>
       <c r="I39">
-        <v>0.0286771510308121</v>
+        <v>0.0140959786863972</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GHDCA</t>
+          <t>GLCA</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1751,28 +1751,28 @@
         </is>
       </c>
       <c r="D40">
-        <v>4.02084455382725</v>
+        <v>4.49364453060249</v>
       </c>
       <c r="E40">
-        <v>1.01947034900022</v>
+        <v>1.06465699673004</v>
       </c>
       <c r="F40">
         <v>45</v>
       </c>
       <c r="G40">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H40">
-        <v>0.00038589889459581</v>
+        <v>0.00017803174137804</v>
       </c>
       <c r="I40">
-        <v>0.0355026983028146</v>
+        <v>0.0185153011033171</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>wMCA</t>
+          <t>Lys_DCA_a</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1786,28 +1786,28 @@
         </is>
       </c>
       <c r="D41">
-        <v>-2.73143524269462</v>
+        <v>1.33609083935223</v>
       </c>
       <c r="E41">
-        <v>0.6884375910995379</v>
+        <v>0.318238128441892</v>
       </c>
       <c r="F41">
         <v>45</v>
       </c>
       <c r="G41">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H41">
-        <v>0.00039948913440694</v>
+        <v>0.00018922025554688</v>
       </c>
       <c r="I41">
-        <v>0.0367530003654385</v>
+        <v>0.0196789065768761</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>HCA</t>
+          <t>TbMCA</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1821,28 +1821,28 @@
         </is>
       </c>
       <c r="D42">
-        <v>-2.905821842312</v>
+        <v>-3.07838356838709</v>
       </c>
       <c r="E42">
-        <v>0.73483326782571</v>
+        <v>0.720246856317878</v>
       </c>
       <c r="F42">
         <v>45</v>
       </c>
       <c r="G42">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="H42">
-        <v>0.00040330240265472</v>
+        <v>0.00022260807418096</v>
       </c>
       <c r="I42">
-        <v>0.037103821044235</v>
+        <v>0.0231512397148207</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Lys_CA_a</t>
+          <t>Glu_DCA</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1856,28 +1856,28 @@
         </is>
       </c>
       <c r="D43">
-        <v>-3.24592439247163</v>
+        <v>4.14453675934297</v>
       </c>
       <c r="E43">
-        <v>0.867928885387846</v>
+        <v>1.01797610844224</v>
       </c>
       <c r="F43">
         <v>45</v>
       </c>
       <c r="G43">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H43">
-        <v>0.00053985013264318</v>
+        <v>0.00026496332538166</v>
       </c>
       <c r="I43">
-        <v>0.0496662122031734</v>
+        <v>0.0275561858396934</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Lys_HCA</t>
+          <t>THDCA</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1891,127 +1891,127 @@
         </is>
       </c>
       <c r="D44">
-        <v>-3.23130200517868</v>
+        <v>-2.43236725452046</v>
       </c>
       <c r="E44">
-        <v>0.864510744427974</v>
+        <v>0.602796137501093</v>
       </c>
       <c r="F44">
         <v>45</v>
       </c>
       <c r="G44">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H44">
-        <v>0.00054330076187414</v>
+        <v>0.00031170816337839</v>
       </c>
       <c r="I44">
-        <v>0.0499836700924214</v>
+        <v>0.0324176489913528</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>12-oxo LCA</t>
+          <t>GHDCA</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>TIME.POINT.2</t>
+          <t>prepost</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D45">
-        <v>13.0324139227966</v>
+        <v>4.02084455382725</v>
       </c>
       <c r="E45">
-        <v>1.18006515393269</v>
+        <v>1.01947034900022</v>
       </c>
       <c r="F45">
         <v>45</v>
       </c>
       <c r="G45">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="H45">
-        <v>6.58269651074878e-10</v>
+        <v>0.00038589889459581</v>
       </c>
       <c r="I45">
-        <v>1.81682423696666e-07</v>
+        <v>0.0401334850379643</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>12-oxo LCA</t>
+          <t>wMCA</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>TIME.POINT.2</t>
+          <t>prepost</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D46">
-        <v>12.0744075630122</v>
+        <v>-2.73143524269462</v>
       </c>
       <c r="E46">
-        <v>1.08673225956147</v>
+        <v>0.6884375910995379</v>
       </c>
       <c r="F46">
         <v>45</v>
       </c>
       <c r="G46">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="H46">
-        <v>7.04544832323205e-10</v>
+        <v>0.00039948913440694</v>
       </c>
       <c r="I46">
-        <v>1.94454373721205e-07</v>
+        <v>0.0415468699783218</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>HDCA</t>
+          <t>HCA</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>TIME.POINT.2</t>
+          <t>prepost</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>Post</t>
         </is>
       </c>
       <c r="D47">
-        <v>11.9009202978973</v>
+        <v>-2.905821842312</v>
       </c>
       <c r="E47">
-        <v>1.18313509454339</v>
+        <v>0.73483326782571</v>
       </c>
       <c r="F47">
         <v>45</v>
       </c>
       <c r="G47">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="H47">
-        <v>9.40163767870899e-10</v>
+        <v>0.00040330240265472</v>
       </c>
       <c r="I47">
-        <v>2.59485199932368e-07</v>
+        <v>0.0419434498760917</v>
       </c>
     </row>
     <row r="48">
@@ -2027,14 +2027,14 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>6 month</t>
         </is>
       </c>
       <c r="D48">
-        <v>10.8470314874921</v>
+        <v>13.0324139227966</v>
       </c>
       <c r="E48">
-        <v>1.05027302635676</v>
+        <v>1.18006515393269</v>
       </c>
       <c r="F48">
         <v>45</v>
@@ -2043,16 +2043,16 @@
         <v>32</v>
       </c>
       <c r="H48">
-        <v>2.63810905663716e-09</v>
+        <v>6.58269651074878e-10</v>
       </c>
       <c r="I48">
-        <v>7.28118099631855e-07</v>
+        <v>2.05380131135362e-07</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>HDCA</t>
+          <t>12-oxo LCA</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2062,26 +2062,26 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D49">
-        <v>10.6398169485594</v>
+        <v>12.0744075630122</v>
       </c>
       <c r="E49">
-        <v>1.14386046266141</v>
+        <v>1.08673225956147</v>
       </c>
       <c r="F49">
         <v>45</v>
       </c>
       <c r="G49">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H49">
-        <v>4.32345381651789e-09</v>
+        <v>7.04544832323205e-10</v>
       </c>
       <c r="I49">
-        <v>1.19327325335894e-06</v>
+        <v>2.1981798768484e-07</v>
       </c>
     </row>
     <row r="50">
@@ -2097,14 +2097,14 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D50">
-        <v>11.6692168683458</v>
+        <v>11.9009202978973</v>
       </c>
       <c r="E50">
-        <v>1.28394240652025</v>
+        <v>1.18313509454339</v>
       </c>
       <c r="F50">
         <v>45</v>
@@ -2113,16 +2113,16 @@
         <v>34</v>
       </c>
       <c r="H50">
-        <v>4.95413853412976e-09</v>
+        <v>9.40163767870899e-10</v>
       </c>
       <c r="I50">
-        <v>1.36734223541981e-06</v>
+        <v>2.93331095575721e-07</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>LCA</t>
+          <t>12-oxo LCA</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2132,32 +2132,32 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D51">
-        <v>9.736832759348969</v>
+        <v>10.8470314874921</v>
       </c>
       <c r="E51">
-        <v>0.928950936519238</v>
+        <v>1.05027302635676</v>
       </c>
       <c r="F51">
         <v>45</v>
       </c>
       <c r="G51">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="H51">
-        <v>1.77316231847185e-08</v>
+        <v>2.63810905663716e-09</v>
       </c>
       <c r="I51">
-        <v>4.8939279989823e-06</v>
+        <v>8.23090025670793e-07</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>DCA</t>
+          <t>HDCA</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2167,32 +2167,32 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D52">
-        <v>9.4771598234557</v>
+        <v>10.6398169485594</v>
       </c>
       <c r="E52">
-        <v>1.12800694345993</v>
+        <v>1.14386046266141</v>
       </c>
       <c r="F52">
         <v>45</v>
       </c>
       <c r="G52">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="H52">
-        <v>2.21802594705839e-08</v>
+        <v>4.32345381651789e-09</v>
       </c>
       <c r="I52">
-        <v>6.12175161388116e-06</v>
+        <v>1.34891759075358e-06</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>EDCA</t>
+          <t>HDCA</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2206,28 +2206,28 @@
         </is>
       </c>
       <c r="D53">
-        <v>7.21413793821981</v>
+        <v>11.6692168683458</v>
       </c>
       <c r="E53">
-        <v>0.924475662019601</v>
+        <v>1.28394240652025</v>
       </c>
       <c r="F53">
         <v>45</v>
       </c>
       <c r="G53">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H53">
-        <v>3.36759581663605e-08</v>
+        <v>4.95413853412976e-09</v>
       </c>
       <c r="I53">
-        <v>9.294564453915509e-06</v>
+        <v>1.54569122264849e-06</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>EDCA</t>
+          <t>LCA</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2241,28 +2241,28 @@
         </is>
       </c>
       <c r="D54">
-        <v>6.73468949593443</v>
+        <v>9.736832759348969</v>
       </c>
       <c r="E54">
-        <v>0.853802901447768</v>
+        <v>0.928950936519238</v>
       </c>
       <c r="F54">
         <v>45</v>
       </c>
       <c r="G54">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="H54">
-        <v>3.61789849677021e-08</v>
+        <v>1.77316231847185e-08</v>
       </c>
       <c r="I54">
-        <v>9.98539985108579e-06</v>
+        <v>5.53226643363217e-06</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>LCA</t>
+          <t>DCA</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2272,32 +2272,32 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D55">
-        <v>8.90915044198087</v>
+        <v>9.4771598234557</v>
       </c>
       <c r="E55">
-        <v>0.89849794946471</v>
+        <v>1.12800694345993</v>
       </c>
       <c r="F55">
         <v>45</v>
       </c>
       <c r="G55">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H55">
-        <v>4.57645371116796e-08</v>
+        <v>2.21802594705839e-08</v>
       </c>
       <c r="I55">
-        <v>1.26310122428236e-05</v>
+        <v>6.92024095482218e-06</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>LCA</t>
+          <t>EDCA</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2311,28 +2311,28 @@
         </is>
       </c>
       <c r="D56">
-        <v>9.59507246446198</v>
+        <v>7.21413793821981</v>
       </c>
       <c r="E56">
-        <v>1.00732503024954</v>
+        <v>0.924475662019601</v>
       </c>
       <c r="F56">
         <v>45</v>
       </c>
       <c r="G56">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="H56">
-        <v>4.69555891171336e-08</v>
+        <v>3.36759581663605e-08</v>
       </c>
       <c r="I56">
-        <v>1.29597425963289e-05</v>
+        <v>1.05068989479045e-05</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>DCA</t>
+          <t>EDCA</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2342,32 +2342,32 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D57">
-        <v>9.51324908431102</v>
+        <v>6.73468949593443</v>
       </c>
       <c r="E57">
-        <v>1.21827281970879</v>
+        <v>0.853802901447768</v>
       </c>
       <c r="F57">
         <v>45</v>
       </c>
       <c r="G57">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="H57">
-        <v>4.80329196430462e-08</v>
+        <v>3.61789849677021e-08</v>
       </c>
       <c r="I57">
-        <v>1.32570858214807e-05</v>
+        <v>1.12878433099231e-05</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>isoLCA</t>
+          <t>LCA</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2377,32 +2377,32 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D58">
-        <v>13.313131967013</v>
+        <v>8.90915044198087</v>
       </c>
       <c r="E58">
-        <v>1.5974831323346</v>
+        <v>0.89849794946471</v>
       </c>
       <c r="F58">
         <v>45</v>
       </c>
       <c r="G58">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H58">
-        <v>9.07681403862571e-08</v>
+        <v>4.57645371116796e-08</v>
       </c>
       <c r="I58">
-        <v>2.5052006746607e-05</v>
+        <v>1.4278535578844e-05</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DCA</t>
+          <t>LCA</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2412,32 +2412,32 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>6 month</t>
         </is>
       </c>
       <c r="D59">
-        <v>8.500663927480179</v>
+        <v>9.59507246446198</v>
       </c>
       <c r="E59">
-        <v>1.09325531502579</v>
+        <v>1.00732503024954</v>
       </c>
       <c r="F59">
         <v>45</v>
       </c>
       <c r="G59">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H59">
-        <v>1.03055935448789e-07</v>
+        <v>4.69555891171336e-08</v>
       </c>
       <c r="I59">
-        <v>2.84434381838658e-05</v>
+        <v>1.46501438045457e-05</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>isoLCA</t>
+          <t>DCA</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2451,22 +2451,22 @@
         </is>
       </c>
       <c r="D60">
-        <v>13.398588091924</v>
+        <v>9.51324908431102</v>
       </c>
       <c r="E60">
-        <v>1.7302861806195</v>
+        <v>1.21827281970879</v>
       </c>
       <c r="F60">
         <v>45</v>
       </c>
       <c r="G60">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H60">
-        <v>1.98170099848258e-07</v>
+        <v>4.80329196430462e-08</v>
       </c>
       <c r="I60">
-        <v>5.46949475581191e-05</v>
+        <v>1.49862709286304e-05</v>
       </c>
     </row>
     <row r="61">
@@ -2482,14 +2482,14 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D61">
-        <v>12.1434808085659</v>
+        <v>13.313131967013</v>
       </c>
       <c r="E61">
-        <v>1.5460485576897</v>
+        <v>1.5974831323346</v>
       </c>
       <c r="F61">
         <v>45</v>
@@ -2498,16 +2498,16 @@
         <v>40</v>
       </c>
       <c r="H61">
-        <v>2.59076052428772e-07</v>
+        <v>9.07681403862571e-08</v>
       </c>
       <c r="I61">
-        <v>7.1504990470341e-05</v>
+        <v>2.83196598005122e-05</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>3-oxo LCA</t>
+          <t>DCA</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2517,32 +2517,32 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D62">
-        <v>7.80614900105597</v>
+        <v>8.500663927480179</v>
       </c>
       <c r="E62">
-        <v>1.0864848231414</v>
+        <v>1.09325531502579</v>
       </c>
       <c r="F62">
         <v>45</v>
       </c>
       <c r="G62">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H62">
-        <v>2.96549146926771e-07</v>
+        <v>1.03055935448789e-07</v>
       </c>
       <c r="I62">
-        <v>8.18475645517887e-05</v>
+        <v>3.21534518600222e-05</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>EDCA</t>
+          <t>isoLCA</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2552,32 +2552,32 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>6 month</t>
         </is>
       </c>
       <c r="D63">
-        <v>5.52323597779199</v>
+        <v>13.398588091924</v>
       </c>
       <c r="E63">
-        <v>0.826453986275283</v>
+        <v>1.7302861806195</v>
       </c>
       <c r="F63">
         <v>45</v>
       </c>
       <c r="G63">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H63">
-        <v>6.639291982894e-07</v>
+        <v>1.98170099848258e-07</v>
       </c>
       <c r="I63">
-        <v>0.00018324445872787</v>
+        <v>6.182907115265641e-05</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>3-oxo LCA</t>
+          <t>isoLCA</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2587,26 +2587,26 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D64">
-        <v>7.551490811024</v>
+        <v>12.1434808085659</v>
       </c>
       <c r="E64">
-        <v>1.17751846156711</v>
+        <v>1.5460485576897</v>
       </c>
       <c r="F64">
         <v>45</v>
       </c>
       <c r="G64">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H64">
-        <v>1.45776759998318e-06</v>
+        <v>2.59076052428772e-07</v>
       </c>
       <c r="I64">
-        <v>0.00040234385759535</v>
+        <v>8.08317283577768e-05</v>
       </c>
     </row>
     <row r="65">
@@ -2622,14 +2622,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D65">
-        <v>6.68946072542034</v>
+        <v>7.80614900105597</v>
       </c>
       <c r="E65">
-        <v>1.05116985574388</v>
+        <v>1.0864848231414</v>
       </c>
       <c r="F65">
         <v>45</v>
@@ -2638,16 +2638,16 @@
         <v>43</v>
       </c>
       <c r="H65">
-        <v>2.07232789436461e-06</v>
+        <v>2.96549146926771e-07</v>
       </c>
       <c r="I65">
-        <v>0.00057196249884463</v>
+        <v>9.25233338411525e-05</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7-keto DCA</t>
+          <t>EDCA</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2657,32 +2657,32 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D66">
-        <v>-7.00691298215236</v>
+        <v>5.52323597779199</v>
       </c>
       <c r="E66">
-        <v>1.25289342471838</v>
+        <v>0.826453986275283</v>
       </c>
       <c r="F66">
         <v>45</v>
       </c>
       <c r="G66">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H66">
-        <v>3.42709062047043e-06</v>
+        <v>6.639291982894e-07</v>
       </c>
       <c r="I66">
-        <v>0.00094587701124984</v>
+        <v>0.00020714590986629</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>THCA</t>
+          <t>3-oxo LCA</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2692,32 +2692,32 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>6 month</t>
         </is>
       </c>
       <c r="D67">
-        <v>-4.54556880761489</v>
+        <v>7.551490811024</v>
       </c>
       <c r="E67">
-        <v>0.920941325459624</v>
+        <v>1.17751846156711</v>
       </c>
       <c r="F67">
         <v>45</v>
       </c>
       <c r="G67">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H67">
-        <v>1.37867755983895e-05</v>
+        <v>1.45776759998318e-06</v>
       </c>
       <c r="I67">
-        <v>0.0038051500651555</v>
+        <v>0.00045482349119475</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>THCA</t>
+          <t>3-oxo LCA</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -2727,32 +2727,32 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D68">
-        <v>-4.44556880761489</v>
+        <v>6.68946072542034</v>
       </c>
       <c r="E68">
-        <v>0.9478357736573479</v>
+        <v>1.05116985574388</v>
       </c>
       <c r="F68">
         <v>45</v>
       </c>
       <c r="G68">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H68">
-        <v>3.02003682911145e-05</v>
+        <v>2.07232789436461e-06</v>
       </c>
       <c r="I68">
-        <v>0.008335301648347591</v>
+        <v>0.00064656630304175</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>TCA</t>
+          <t>7-keto DCA</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2766,28 +2766,28 @@
         </is>
       </c>
       <c r="D69">
-        <v>-7.95902661968295</v>
+        <v>-7.00691298215236</v>
       </c>
       <c r="E69">
-        <v>1.63927834581668</v>
+        <v>1.25289342471838</v>
       </c>
       <c r="F69">
         <v>45</v>
       </c>
       <c r="G69">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H69">
-        <v>3.76389872521912e-05</v>
+        <v>3.42709062047043e-06</v>
       </c>
       <c r="I69">
-        <v>0.0103883604816048</v>
+        <v>0.00106925227358678</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>TCA</t>
+          <t>THCA</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2801,28 +2801,28 @@
         </is>
       </c>
       <c r="D70">
-        <v>-7.13638459310861</v>
+        <v>-4.54556880761489</v>
       </c>
       <c r="E70">
-        <v>1.46236048842219</v>
+        <v>0.920941325459624</v>
       </c>
       <c r="F70">
         <v>45</v>
       </c>
       <c r="G70">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="H70">
-        <v>3.76597939380561e-05</v>
+        <v>1.37867755983895e-05</v>
       </c>
       <c r="I70">
-        <v>0.0103941031269035</v>
+        <v>0.00430147398669752</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Ile_Leu_CA</t>
+          <t>Phe_LCA</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2832,32 +2832,32 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>6 month</t>
         </is>
       </c>
       <c r="D71">
-        <v>-6.10058521082559</v>
+        <v>3.7533008234672</v>
       </c>
       <c r="E71">
-        <v>1.33271326638857</v>
+        <v>0.7617813618875779</v>
       </c>
       <c r="F71">
         <v>45</v>
       </c>
       <c r="G71">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H71">
-        <v>4.31474313102014e-05</v>
+        <v>2.64114544279239e-05</v>
       </c>
       <c r="I71">
-        <v>0.0119086910416156</v>
+        <v>0.008240373781512241</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>THCA</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2867,32 +2867,32 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D72">
-        <v>-6.25216902572165</v>
+        <v>-4.44556880761489</v>
       </c>
       <c r="E72">
-        <v>1.32881437275071</v>
+        <v>0.9478357736573479</v>
       </c>
       <c r="F72">
         <v>45</v>
       </c>
       <c r="G72">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="H72">
-        <v>4.41643241677876e-05</v>
+        <v>3.02003682911145e-05</v>
       </c>
       <c r="I72">
-        <v>0.0121893534703094</v>
+        <v>0.00942251490682772</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>GHDCA</t>
+          <t>Phe_LCA</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2906,28 +2906,28 @@
         </is>
       </c>
       <c r="D73">
-        <v>5.80674687717921</v>
+        <v>3.40382866248224</v>
       </c>
       <c r="E73">
-        <v>1.23608999127454</v>
+        <v>0.70232083798512</v>
       </c>
       <c r="F73">
         <v>45</v>
       </c>
       <c r="G73">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H73">
-        <v>4.78380267500087e-05</v>
+        <v>3.43108304228955e-05</v>
       </c>
       <c r="I73">
-        <v>0.0132032953830024</v>
+        <v>0.0107049790919434</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Phe_DCA</t>
+          <t>TCA</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2941,28 +2941,28 @@
         </is>
       </c>
       <c r="D74">
-        <v>6.64065918714647</v>
+        <v>-7.95902661968295</v>
       </c>
       <c r="E74">
-        <v>1.41108798290174</v>
+        <v>1.63927834581668</v>
       </c>
       <c r="F74">
         <v>45</v>
       </c>
       <c r="G74">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="H74">
-        <v>4.78682646906406e-05</v>
+        <v>3.76389872521912e-05</v>
       </c>
       <c r="I74">
-        <v>0.0132116410546168</v>
+        <v>0.0117433640226836</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Val_CA</t>
+          <t>TCA</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2972,32 +2972,32 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D75">
-        <v>-5.84339546717036</v>
+        <v>-7.13638459310861</v>
       </c>
       <c r="E75">
-        <v>1.28629006191012</v>
+        <v>1.46236048842219</v>
       </c>
       <c r="F75">
         <v>45</v>
       </c>
       <c r="G75">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="H75">
-        <v>4.8144262288321e-05</v>
+        <v>3.76597939380561e-05</v>
       </c>
       <c r="I75">
-        <v>0.0132878163915766</v>
+        <v>0.0117498557086735</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>TCDCA</t>
+          <t>Ile_Leu_CA</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3007,32 +3007,32 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D76">
-        <v>-6.4384365413364</v>
+        <v>-6.10058521082559</v>
       </c>
       <c r="E76">
-        <v>1.34768443484017</v>
+        <v>1.33271326638857</v>
       </c>
       <c r="F76">
         <v>45</v>
       </c>
       <c r="G76">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="H76">
-        <v>5.09307989505044e-05</v>
+        <v>4.31474313102014e-05</v>
       </c>
       <c r="I76">
-        <v>0.0140569005103392</v>
+        <v>0.0134619985687828</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7-keto DCA</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3042,32 +3042,32 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>6 month</t>
         </is>
       </c>
       <c r="D77">
-        <v>-5.19615591186174</v>
+        <v>-6.25216902572165</v>
       </c>
       <c r="E77">
-        <v>1.12047899224914</v>
+        <v>1.32881437275071</v>
       </c>
       <c r="F77">
         <v>45</v>
       </c>
       <c r="G77">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H77">
-        <v>5.96302643154319e-05</v>
+        <v>4.41643241677876e-05</v>
       </c>
       <c r="I77">
-        <v>0.0164579529510592</v>
+        <v>0.0137792691403497</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>THCA</t>
+          <t>GHDCA</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3077,32 +3077,32 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D78">
-        <v>-4.54556880761489</v>
+        <v>5.80674687717921</v>
       </c>
       <c r="E78">
-        <v>1.01813894349405</v>
+        <v>1.23608999127454</v>
       </c>
       <c r="F78">
         <v>45</v>
       </c>
       <c r="G78">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H78">
-        <v>6.15728356918681e-05</v>
+        <v>4.78380267500087e-05</v>
       </c>
       <c r="I78">
-        <v>0.0169941026509556</v>
+        <v>0.0149254643460027</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Ala_DCA</t>
+          <t>Phe_DCA</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3112,32 +3112,32 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>6 month</t>
         </is>
       </c>
       <c r="D79">
-        <v>4.41202337505393</v>
+        <v>6.64065918714647</v>
       </c>
       <c r="E79">
-        <v>0.957042656256704</v>
+        <v>1.41108798290174</v>
       </c>
       <c r="F79">
         <v>45</v>
       </c>
       <c r="G79">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H79">
-        <v>6.38821415150194e-05</v>
+        <v>4.78682646906406e-05</v>
       </c>
       <c r="I79">
-        <v>0.0176314710581454</v>
+        <v>0.0149348985834799</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>Val_CA</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3147,32 +3147,32 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D80">
-        <v>-5.41632966013603</v>
+        <v>-5.84339546717036</v>
       </c>
       <c r="E80">
-        <v>1.19607475680274</v>
+        <v>1.28629006191012</v>
       </c>
       <c r="F80">
         <v>45</v>
       </c>
       <c r="G80">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H80">
-        <v>8.35452350922207e-05</v>
+        <v>4.8144262288321e-05</v>
       </c>
       <c r="I80">
-        <v>0.0230584848854529</v>
+        <v>0.0150210098339561</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>TCDCA</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3182,32 +3182,32 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>6 month</t>
         </is>
       </c>
       <c r="D81">
-        <v>-5.54660780495289</v>
+        <v>-6.4384365413364</v>
       </c>
       <c r="E81">
-        <v>1.23289257891194</v>
+        <v>1.34768443484017</v>
       </c>
       <c r="F81">
         <v>45</v>
       </c>
       <c r="G81">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H81">
-        <v>8.73189231857512e-05</v>
+        <v>5.09307989505044e-05</v>
       </c>
       <c r="I81">
-        <v>0.0241000227992673</v>
+        <v>0.0158904092725574</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Ala_CA</t>
+          <t>7-keto DCA</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3217,32 +3217,32 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D82">
-        <v>-4.31556274049233</v>
+        <v>-5.19615591186174</v>
       </c>
       <c r="E82">
-        <v>0.967119044759749</v>
+        <v>1.12047899224914</v>
       </c>
       <c r="F82">
         <v>45</v>
       </c>
       <c r="G82">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H82">
-        <v>0.00011030706666343</v>
+        <v>5.96302643154319e-05</v>
       </c>
       <c r="I82">
-        <v>0.030444750399109</v>
+        <v>0.0186046424664148</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Ala_DCA</t>
+          <t>THCA</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3256,28 +3256,28 @@
         </is>
       </c>
       <c r="D83">
-        <v>4.55656186958944</v>
+        <v>-4.54556880761489</v>
       </c>
       <c r="E83">
-        <v>1.03681226283981</v>
+        <v>1.01813894349405</v>
       </c>
       <c r="F83">
         <v>45</v>
       </c>
       <c r="G83">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H83">
-        <v>0.00011425178861924</v>
+        <v>6.15728356918681e-05</v>
       </c>
       <c r="I83">
-        <v>0.0315334936589103</v>
+        <v>0.0192107247358628</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Val_CA</t>
+          <t>Ala_DCA</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3287,32 +3287,32 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D84">
-        <v>-5.84339546717036</v>
+        <v>4.41202337505393</v>
       </c>
       <c r="E84">
-        <v>1.38169716849441</v>
+        <v>0.957042656256704</v>
       </c>
       <c r="F84">
         <v>45</v>
       </c>
       <c r="G84">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H84">
-        <v>0.00012816382487694</v>
+        <v>6.38821415150194e-05</v>
       </c>
       <c r="I84">
-        <v>0.0353732156660356</v>
+        <v>0.0199312281526861</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7-keto DCA</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -3322,32 +3322,32 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2 month</t>
+          <t>2 week</t>
         </is>
       </c>
       <c r="D85">
-        <v>-5.04518300980729</v>
+        <v>-5.41632966013603</v>
       </c>
       <c r="E85">
-        <v>1.15740770712532</v>
+        <v>1.19607475680274</v>
       </c>
       <c r="F85">
         <v>45</v>
       </c>
       <c r="G85">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H85">
-        <v>0.00012915185789265</v>
+        <v>8.35452350922207e-05</v>
       </c>
       <c r="I85">
-        <v>0.0356459127783731</v>
+        <v>0.0260661133487729</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Val_CA</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -3357,32 +3357,32 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D86">
-        <v>-5.26786881688471</v>
+        <v>-5.54660780495289</v>
       </c>
       <c r="E86">
-        <v>1.24979211321612</v>
+        <v>1.23289257891194</v>
       </c>
       <c r="F86">
         <v>45</v>
       </c>
       <c r="G86">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="H86">
-        <v>0.00013388551626987</v>
+        <v>8.73189231857512e-05</v>
       </c>
       <c r="I86">
-        <v>0.0369524024904865</v>
+        <v>0.0272435040339544</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Ile_Leu_CA</t>
+          <t>Ala_CA</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -3392,32 +3392,32 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>6 month</t>
+          <t>2 month</t>
         </is>
       </c>
       <c r="D87">
-        <v>-5.97558521082559</v>
+        <v>-4.31556274049233</v>
       </c>
       <c r="E87">
-        <v>1.4315636893358</v>
+        <v>0.967119044759749</v>
       </c>
       <c r="F87">
         <v>45</v>
       </c>
       <c r="G87">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H87">
-        <v>0.00015183268108937</v>
+        <v>0.00011030706666343</v>
       </c>
       <c r="I87">
-        <v>0.0419058199806677</v>
+        <v>0.0344158047989927</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>TCDCA</t>
+          <t>Ala_DCA</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -3427,32 +3427,32 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2 week</t>
+          <t>6 month</t>
         </is>
       </c>
       <c r="D88">
-        <v>-5.24013234913862</v>
+        <v>4.55656186958944</v>
       </c>
       <c r="E88">
-        <v>1.19988005658004</v>
+        <v>1.03681226283981</v>
       </c>
       <c r="F88">
         <v>45</v>
       </c>
       <c r="G88">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="H88">
-        <v>0.00016077492012957</v>
+        <v>0.00011425178861924</v>
       </c>
       <c r="I88">
-        <v>0.0443738779557637</v>
+        <v>0.0356465580492029</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>aMCA</t>
+          <t>Val_CA</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -3466,28 +3466,28 @@
         </is>
       </c>
       <c r="D89">
-        <v>6.80916450829086</v>
+        <v>-5.84339546717036</v>
       </c>
       <c r="E89">
-        <v>1.56700291510065</v>
+        <v>1.38169716849441</v>
       </c>
       <c r="F89">
         <v>45</v>
       </c>
       <c r="G89">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="H89">
-        <v>0.00017610010439449</v>
+        <v>0.00012816382487694</v>
       </c>
       <c r="I89">
-        <v>0.0486036288128795</v>
+        <v>0.0399871133616055</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Ser_CDCA</t>
+          <t>7-keto DCA</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -3497,26 +3497,131 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
+          <t>2 month</t>
+        </is>
+      </c>
+      <c r="D90">
+        <v>-5.04518300980729</v>
+      </c>
+      <c r="E90">
+        <v>1.15740770712532</v>
+      </c>
+      <c r="F90">
+        <v>45</v>
+      </c>
+      <c r="G90">
+        <v>42</v>
+      </c>
+      <c r="H90">
+        <v>0.00012915185789265</v>
+      </c>
+      <c r="I90">
+        <v>0.0402953796625087</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Leu_LCA</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>TIME.POINT.2</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2 month</t>
+        </is>
+      </c>
+      <c r="D91">
+        <v>4.77981232423534</v>
+      </c>
+      <c r="E91">
+        <v>1.08388228562827</v>
+      </c>
+      <c r="F91">
+        <v>45</v>
+      </c>
+      <c r="G91">
+        <v>22</v>
+      </c>
+      <c r="H91">
+        <v>0.00013279995177981</v>
+      </c>
+      <c r="I91">
+        <v>0.0414335849553011</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Val_CA</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>TIME.POINT.2</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
           <t>2 week</t>
         </is>
       </c>
-      <c r="D90">
-        <v>-3.79484990533002</v>
-      </c>
-      <c r="E90">
-        <v>0.861389485684584</v>
-      </c>
-      <c r="F90">
-        <v>45</v>
-      </c>
-      <c r="G90">
-        <v>12</v>
-      </c>
-      <c r="H90">
-        <v>0.00017818256316173</v>
-      </c>
-      <c r="I90">
-        <v>0.0491783874326401</v>
+      <c r="D92">
+        <v>-5.26786881688471</v>
+      </c>
+      <c r="E92">
+        <v>1.24979211321612</v>
+      </c>
+      <c r="F92">
+        <v>45</v>
+      </c>
+      <c r="G92">
+        <v>13</v>
+      </c>
+      <c r="H92">
+        <v>0.00013388551626987</v>
+      </c>
+      <c r="I92">
+        <v>0.0417722810762021</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Ile_Leu_CA</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>TIME.POINT.2</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>6 month</t>
+        </is>
+      </c>
+      <c r="D93">
+        <v>-5.97558521082559</v>
+      </c>
+      <c r="E93">
+        <v>1.4315636893358</v>
+      </c>
+      <c r="F93">
+        <v>45</v>
+      </c>
+      <c r="G93">
+        <v>14</v>
+      </c>
+      <c r="H93">
+        <v>0.00015183268108937</v>
+      </c>
+      <c r="I93">
+        <v>0.0473717964998852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>